<commit_message>
Changes in Shift Tag has been implemented
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <x:si>
     <x:t>Shifts</x:t>
   </x:si>
@@ -105,18 +105,6 @@
     <x:t>A
 Nurse
 R  1.0
-A 0.0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>B
-Nurse
-R  1.0
-A 0.0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A
-Nurse
-R  1.0
 A 0.0
 B
 Nurse
@@ -124,6 +112,18 @@
 A 0.0</x:t>
   </x:si>
   <x:si>
+    <x:t>B
+Nurse
+R  1.0
+A 0.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C
+Nurse
+R  1.0
+A 0.0</x:t>
+  </x:si>
+  <x:si>
     <x:t>2p-6p</x:t>
   </x:si>
   <x:si>
@@ -140,17 +140,11 @@
     <x:t>A/B Wing
 CNA
 R  3.0
-A 2.0
-Primrose
-CNA
-R  1.0
-A 0.0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A/B Wing
-CNA
-R  3.0
 A 2.5
+C/D Wing
+CNA
+R  2.0
+A 1.0
 Primrose
 CNA
 R  1.0
@@ -191,6 +185,12 @@
     <x:t>A
 Nurse
 R  1.0
+A 0.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A
+Nurse
+R  1.0
 A 0.0
 C
 Nurse
@@ -211,7 +211,17 @@
 A 0.0</x:t>
   </x:si>
   <x:si>
-    <x:t>JCR
+    <x:t>C/D Wing
+CNA
+R  1.0
+A 0.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C/D Wing
+CNA
+R  1.0
+A 0.0
+JCR
 CNA
 R  1.0
 A 0.0
@@ -221,7 +231,11 @@
 A 0.0</x:t>
   </x:si>
   <x:si>
-    <x:t>JCR
+    <x:t>C/D Wing
+CNA
+R  1.0
+A 0.0
+JCR
 CNA
 R  1.0
 A 0.0</x:t>
@@ -290,12 +304,120 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="112">
+  <x:cellStyleXfs count="148">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -996,16 +1118,20 @@
       <x:c r="C3" s="5" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D3" s="5" t="s"/>
-      <x:c r="E3" s="5" t="s"/>
+      <x:c r="D3" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E3" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
       <x:c r="F3" s="5" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="G3" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="H3" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1032,36 +1158,36 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="B5" s="5" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C5" s="5" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="C5" s="5" t="s">
+      <x:c r="D5" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="D5" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
       <x:c r="E5" s="5" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F5" s="5" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="G5" s="5" t="s">
-        <x:v>20</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="H5" s="5" t="s">
-        <x:v>20</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A6" s="3" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B6" s="5" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B6" s="5" t="s">
+      <x:c r="C6" s="5" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="C6" s="5" t="s">
-        <x:v>14</x:v>
       </x:c>
       <x:c r="D6" s="5" t="s">
         <x:v>25</x:v>
@@ -1084,15 +1210,17 @@
       <x:c r="B7" s="5" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C7" s="5" t="s"/>
+      <x:c r="C7" s="5" t="s">
+        <x:v>28</x:v>
+      </x:c>
       <x:c r="D7" s="5" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="E7" s="5" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F7" s="5" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G7" s="5" t="s">
         <x:v>27</x:v>
@@ -1103,16 +1231,16 @@
     </x:row>
     <x:row r="8" spans="1:8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A8" s="3" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E8" s="5" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F8" s="5" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G8" s="5" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>